<commit_message>
First person removed from first 2 chapters
</commit_message>
<xml_diff>
--- a/ResponseDocument.xlsx
+++ b/ResponseDocument.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t xml:space="preserve">REVIEWER COMMENTS</t>
   </si>
@@ -37,31 +37,82 @@
     <t xml:space="preserve">The text switches from first to third person which becomes quite confusing as a reader. Given that the published work is in 3 rd person, I would suggest keeping the entire thesis the same.</t>
   </si>
   <si>
+    <t xml:space="preserve">I agree, or, there is aggreement</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sentences with I, we, us, my, our, ours are restructured to 3</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> person.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Page v- there are some problems with the formatting of the title/abstract in the version of the thesis I was sent.</t>
   </si>
   <si>
+    <t xml:space="preserve">Some issues I would like to blame on the latex template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’ve changed the abstract so that it does not start at the end of the page. However I also removed the extras such as school and department names.</t>
+  </si>
+  <si>
     <t xml:space="preserve">The abstract needs some re-structuring. E.g. the aims come before the need/background. I suggest starting with the need/gaps, following with the aims/approach, and then following with key results. It is also lacking key contribution- why is this work important?</t>
   </si>
   <si>
+    <t xml:space="preserve">The abstract is somewhat reordered, with background more at the start and some additional notes on importance</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abstract- typo “A”- 3 rd paragraph</t>
   </si>
   <si>
+    <t xml:space="preserve">fixed</t>
+  </si>
+  <si>
     <t xml:space="preserve">As with the Abstract, Chapter 1 could also do with some restructuring. The chapter contains a comprehensive introduction to ozone, and review of literature, however the gaps in knowledge that this thesis fills are hidden throughout and it is difficult to assess the context to the current study for some of the sections. Again, I suggest bearing in mind: need, gaps, aims/objectives structure while also introducing key background material and literature.</t>
   </si>
   <si>
     <t xml:space="preserve">Page 31- typo “..”</t>
   </si>
   <si>
-    <t xml:space="preserve">Chapter 2, called “Data and Modelling” details the datasets and modelling undertaken project on page 30 to see how and why that section fit within the thesis. This is also quite a long chapter. One suggestion would be to split the first half into a data and methods chapter, and the second half into results to meet Aim 2. I also suggest moving Fig 2.37 to earlier in the chapter, and then reefing to it throughout. in the thesis, while also including results linked to Aim 2- calculation of vertical columns of HCHO. Once again, although the material presented is relevant, and the analyses appropriate, I am going to take issue with the structure of the chapter. As I read each section I found that although each contained interesting and relevant material, I kept having to go back to the explanation of the aims of the</t>
+    <t xml:space="preserve">Chapter 2, called “Data and Modelling” details the datasets and modelling undertaken in the thesis, while also including results linked to Aim 2- calculation of vertical columns of HCHO. Once again, although the material presented is relevant, and the analyses appropriate, I am going to take issue with the structure of the chapter. As I read each section I found that although each contained interesting and relevant material, I kept having to go back to the explanation of the aims of the project on page 30 to see how and why that section fit within the thesis. This is also quite a long chapter. One suggestion would be to split the first half into a data and methods chapter, and the second half into results to meet Aim 2. I also suggest moving Fig 2.37 to earlier in the chapter, and then reefing to it throughout.</t>
   </si>
   <si>
     <t xml:space="preserve">Chapter 3 implements a top-down technique using satellite measurements of HCHO to calculate surface isoprene emissions. This chapter is clearly structured and easy to read and interpret. Well done. I have no suggestions for revisions to this chapter, beyond the use of 1 st person mentioned above, and would suggest that it is ready to submit to a journal if this hasn’t already taken place.</t>
   </si>
   <si>
+    <t xml:space="preserve">Thanks!</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chapter 4 looks at stratospheric ozone intrusions and has been published in Atmospheric Chemistry and Physics. My only suggestion for this chapter would be to move the contribution of authors section to the beginning of the chapter, and to make clear how much of the work, perhaps as a percentage, can be contributed to the candidate.</t>
   </si>
   <si>
     <t xml:space="preserve">Chapter 5 is clearly written and does a good job of synthesizing the work. No revisions suggested.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks</t>
   </si>
   <si>
     <t xml:space="preserve">REVIEWER 2: T. Butler</t>
@@ -92,11 +143,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -134,8 +186,15 @@
       <charset val="1"/>
     </font>
     <font>
+      <vertAlign val="superscript"/>
       <sz val="12"/>
-      <name val=""/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
@@ -196,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,7 +284,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,16 +311,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="59.0459183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="57.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.9081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="58.3163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="56.9642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,124 +338,265 @@
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="44.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="44.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="44.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="86.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="143.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="72.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="72.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="286.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="257.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7"/>
-    </row>
-    <row r="31" customFormat="false" ht="229.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="A30" s="8"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="200.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7"/>
-    </row>
-    <row r="34" customFormat="false" ht="286.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="A33" s="8"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="243.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7"/>
-    </row>
-    <row r="37" customFormat="false" ht="143.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="A36" s="8"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="129.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7"/>
-    </row>
-    <row r="40" customFormat="false" ht="186.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="A39" s="8"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7"/>
-    </row>
-    <row r="43" customFormat="false" ht="44.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="A42" s="8"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
chap 3 3rd personed, chapman update
</commit_message>
<xml_diff>
--- a/ResponseDocument.xlsx
+++ b/ResponseDocument.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t xml:space="preserve">REVIEWER COMMENTS</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">CHANGES TO THESIS</t>
   </si>
   <si>
-    <t xml:space="preserve">REVIEWER 1:</t>
+    <t xml:space="preserve">REVIEWER 1: M Hart</t>
   </si>
   <si>
     <t xml:space="preserve">The text switches from first to third person which becomes quite confusing as a reader. Given that the published work is in 3 rd person, I would suggest keeping the entire thesis the same.</t>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t xml:space="preserve">I noticed several small apparent errors of understanding in Chapter 1 which the candidate should revisit while revising their thesis. For example, on page 3, the hydroperoxyl radical (HO 2 ) is referred to as “hydrogen dioxide”, a name which is never used in the relevant atmospheric chemistry literature. I was also not convinced by some aspects of the candidate’s description of ozone chemistry. For example the photolysis reaction of ozone in Equation Set 1.2 (page 4) is claimed to proceed at wavelengths less than 1180 nm. Does the candidate have a reference describing how quickly the reaction proceeds at such low photon energies? The absorption cross section for ozone photolysis used in the MCM (Master Chemical Mechanism) is only defined below 350 nm, with wavelength-dependent quantum yields for O( 1 D) and O( 3 P) below 350 nm (http://mcm.leeds.ac.uk/MCMv3.3.1/parameters/photolysis.htt). Significant amounts of ozone photolysis at lower photon energies would result in a much shorter lifetime for tropospheric ozone than predicted by the MCM (or any other model which I have used). Furthermore, the high abundance of “M” at lower altitudes is given as a reason for the existence of the ozone-layer, but M are actually required to stabilise ozone produced by photolysis in the stratosphere (Equation Set 1.2), where they are less abundant. The candidate should rethink and revise their text here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemistry is not my strongest suit, so I do not pick up errors as readily as I should – thanks for pointing these out. I had </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low wavelengths discussed in equation set 1.2 are updated to 350nm, with reference updated</t>
   </si>
   <si>
     <t xml:space="preserve">I also think that the candidate should give a better overview of the different kinds of sources of VOC in Section 1.3. The candidate primarily focuses on biogenic isoprene, which is reasonable given the focus of the thesis, but anthropogenic and pyrogenic VOC are barely mentioned, and not until later in the text. Also, “reactivity” is listed as one of the fundamental properties of VOC near the beginning of Section 1.3, but I miss some discussion about what determines the reactivity of different VOC, and what this means for their atmospheric lifetimes. This is especially important, since the atmospheric lifetimes of both isoprene and HCHO are important concepts which are drawn upon in several places later in the thesis.</t>
@@ -311,16 +317,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.9081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="58.3163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="56.9642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="83.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="57.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="56.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,12 +546,16 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="243.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="242.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>
@@ -559,7 +569,7 @@
     </row>
     <row r="37" customFormat="false" ht="129.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -576,7 +586,7 @@
     </row>
     <row r="40" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -593,7 +603,7 @@
     </row>
     <row r="43" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>

</xml_diff>

<commit_message>
added biogenic emissions modelling section 1.3.2
</commit_message>
<xml_diff>
--- a/ResponseDocument.xlsx
+++ b/ResponseDocument.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">REVIEWER COMMENTS</t>
   </si>
@@ -127,16 +127,28 @@
     <t xml:space="preserve">I noticed several small apparent errors of understanding in Chapter 1 which the candidate should revisit while revising their thesis. For example, on page 3, the hydroperoxyl radical (HO 2 ) is referred to as “hydrogen dioxide”, a name which is never used in the relevant atmospheric chemistry literature. I was also not convinced by some aspects of the candidate’s description of ozone chemistry. For example the photolysis reaction of ozone in Equation Set 1.2 (page 4) is claimed to proceed at wavelengths less than 1180 nm. Does the candidate have a reference describing how quickly the reaction proceeds at such low photon energies? The absorption cross section for ozone photolysis used in the MCM (Master Chemical Mechanism) is only defined below 350 nm, with wavelength-dependent quantum yields for O( 1 D) and O( 3 P) below 350 nm (http://mcm.leeds.ac.uk/MCMv3.3.1/parameters/photolysis.htt). Significant amounts of ozone photolysis at lower photon energies would result in a much shorter lifetime for tropospheric ozone than predicted by the MCM (or any other model which I have used). Furthermore, the high abundance of “M” at lower altitudes is given as a reason for the existence of the ozone-layer, but M are actually required to stabilise ozone produced by photolysis in the stratosphere (Equation Set 1.2), where they are less abundant. The candidate should rethink and revise their text here.</t>
   </si>
   <si>
-    <t xml:space="preserve">Chemistry is not my strongest suit, so I do not pick up errors as readily as I should – thanks for pointing these out. I had </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low wavelengths discussed in equation set 1.2 are updated to 350nm, with reference updated</t>
+    <t xml:space="preserve">Chemistry is not my strongest suit, so I do not pick up errors as readily as I should – thanks for pointing these out. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low wavelengths discussed in equation set 1.2 are updated to 350nm, updated sentence dealing with M abundance.</t>
   </si>
   <si>
     <t xml:space="preserve">I also think that the candidate should give a better overview of the different kinds of sources of VOC in Section 1.3. The candidate primarily focuses on biogenic isoprene, which is reasonable given the focus of the thesis, but anthropogenic and pyrogenic VOC are barely mentioned, and not until later in the text. Also, “reactivity” is listed as one of the fundamental properties of VOC near the beginning of Section 1.3, but I miss some discussion about what determines the reactivity of different VOC, and what this means for their atmospheric lifetimes. This is especially important, since the atmospheric lifetimes of both isoprene and HCHO are important concepts which are drawn upon in several places later in the thesis.</t>
   </si>
   <si>
+    <t xml:space="preserve">Thanks, it is good to have feedback on what may be missing from the intro. Instead of shuffling pyro and anthro emissions into the intro, I hope it is ok to just mention that they are important and point to the sections where I deal with them specifically.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added to third paragraph in 1.3: “Other major emission sources of VOC (anthropogenic and pyrogenic) are also important.” and “This thesis mostly focuses on biogenic emissions, with influences from pyrogenic and anthropogenic emissions removed (Section 2.7)”. Added to first paragraph in 1.3: “These properties are largely dictated by the chemical makeup of the individual compounds. A compound's atmospheric lifetime is strongly related to its reactivity (and the concentration of reactants), with more reactive compounds having shorter atmospheric lifetimes.”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Given their importance in the thesis, I would also like to see more understanding of biogenic isoprene emissions demonstrated by the candidate in Chapter 1, especially how they are modelled, and the basis (or lack thereof) that this emissions modelling has in actual measured data. BVOC emission models, specifically MEGAN, are mentioned in several places in the thesis. In many of these cases literature references are given, and particular aspects of the potential shortcomings in these models are described, such as a poor representation of soil moisture, or an over-reliance on measurements from younger trees. Instead of scattering this information throughout the thesis it should be collected in one place where the candidate can demonstrate an understanding of how these models work and what their known shortcomings are. The results in subsequent chapters can then be related back to the material from the introduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fair point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Section 1.3.2: Biogenic emissions modelling, drawing sentences from several sections in chapter 1 and 3</t>
   </si>
   <si>
     <t xml:space="preserve">As a matter of style, tables and figures should not be presented in the conclusions chapter. Figure 5.2 is particularly superfluous, since it is exactly the same as Figure 3.7</t>
@@ -317,16 +329,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="83.8316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="57.6428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="56.2908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="82.8826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="55.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,12 +579,16 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="129.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="157.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8"/>
@@ -584,12 +600,16 @@
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="171.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8"/>
@@ -603,7 +623,7 @@
     </row>
     <row r="43" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>

</xml_diff>

<commit_message>
conclusions 3rd personed, and figures removed
</commit_message>
<xml_diff>
--- a/ResponseDocument.xlsx
+++ b/ResponseDocument.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t xml:space="preserve">REVIEWER COMMENTS</t>
   </si>
@@ -66,7 +66,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> person.</t>
+      <t xml:space="preserve"> person. This is performed throughout the thesis except for the Aims in the conclusion chapter</t>
     </r>
   </si>
   <si>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Some issues I would like to blame on the latex template</t>
   </si>
   <si>
-    <t xml:space="preserve">I’ve changed the abstract so that it does not start at the end of the page. However I also removed the extras such as school and department names.</t>
+    <t xml:space="preserve">I’ve changed the abstract so that it does not start at the end of the page. However I also removed the extras such as school and department names from the abstract header.</t>
   </si>
   <si>
     <t xml:space="preserve">The abstract needs some re-structuring. E.g. the aims come before the need/background. I suggest starting with the need/gaps, following with the aims/approach, and then following with key results. It is also lacking key contribution- why is this work important?</t>
@@ -145,13 +145,19 @@
     <t xml:space="preserve">Given their importance in the thesis, I would also like to see more understanding of biogenic isoprene emissions demonstrated by the candidate in Chapter 1, especially how they are modelled, and the basis (or lack thereof) that this emissions modelling has in actual measured data. BVOC emission models, specifically MEGAN, are mentioned in several places in the thesis. In many of these cases literature references are given, and particular aspects of the potential shortcomings in these models are described, such as a poor representation of soil moisture, or an over-reliance on measurements from younger trees. Instead of scattering this information throughout the thesis it should be collected in one place where the candidate can demonstrate an understanding of how these models work and what their known shortcomings are. The results in subsequent chapters can then be related back to the material from the introduction</t>
   </si>
   <si>
-    <t xml:space="preserve">Fair point.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Added Section 1.3.2: Biogenic emissions modelling, drawing sentences from several sections in chapter 1 and 3</t>
+    <t xml:space="preserve">Fair point, I like the idea of having bvoc emission modelling introduced in one spot. I have left the subsection in Chapter 2 that refers to how MEGAN is implemented within GEOS-Chem, and also several sentences in chapter 3 that are relevant to the surrounding text.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Section 1.3.2: Biogenic emissions modelling, drawing sentences from several sections in chapters 1 and 2, and references to the section are added in chapters 1 2 and 3. </t>
   </si>
   <si>
     <t xml:space="preserve">As a matter of style, tables and figures should not be presented in the conclusions chapter. Figure 5.2 is particularly superfluous, since it is exactly the same as Figure 3.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK it seems fair to have no figures or new material in the conclusions, however I would like to keep the table as it is much clearer than a long list of numbers that I would have otherwise.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 5.1 moved into Chapter 3 results as Figure 3.21, with some text added there, and some text replaced in the Conclusions chapter. Figure 5.2 removed, sentence now references original figure.</t>
   </si>
 </sst>
 </file>
@@ -330,15 +336,15 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="82.8826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="56.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="55.6173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="81.9387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="54.9438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,7 +386,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="44.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -621,12 +627,16 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
filtering to ch3, ch2 intro dupe removed
</commit_message>
<xml_diff>
--- a/ResponseDocument.xlsx
+++ b/ResponseDocument.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t xml:space="preserve">REVIEWER COMMENTS</t>
   </si>
@@ -121,13 +121,16 @@
     <t xml:space="preserve">The novel methodological aspects of the work are described in Chapter 2 of the thesis. I find this chapter somewhat confusing, because it appears to have three distinct purposes. Firstly, the chapter provides some general introductory material, which has substantial overlap with the introductory chapter. Secondly, the work done by the candidate to recalculate the OMI HCHO column measurements is described. These revised data are used in the subsequent chapter on isoprene inverse modelling (and presumably also by Lieschke et all, 2019). Thirdly, several filtering techniques are described, which it seems are only relevant for the isoprene inverse modelling work. I do understand the logic of including all of this material in a chapter called “Data and Modelling”, but I think a separation into distinct chapters would help the reader, and also make it clearer what the candidate has contributed. In particular, for the “middle part” of this text, it would be good to see a section similar to Section 4.9, in which the contributions of different workers (including the candidate) are clearly described. Subsequent work published (and even in preparation) using the new HCHO dataset could also be mentioned here, which would help to show how useful this work has been for colleagues and the wider community. Perhaps the work on filtering the HCHO columns (Section 2.7) could be merged into Chapter 3, especially if this will all be submitted as a standalone paper anyway.</t>
   </si>
   <si>
+    <t xml:space="preserve">Some intro from chapter 2 has been removed or replaced into chapter 1, with references added in chapter 2. Section 2.7: Filtering Data has been moved into Chapter 3 as subsection 3.2.3 under methods.</t>
+  </si>
+  <si>
     <t xml:space="preserve">My main criticism of Chapter 3 is that the work is not described adequately in the context of previous studies. A top-down study by Bauwens et al. (2016) is mentioned in passing in Section 3.1.2, but almost no details are given. This study appears to be highly relevant, given that it seems to use an almost identical method. Chapter 3 must include a comparative discussion of the method used in this thesis and the method of Bauwens et al. (2016), and how the results of the two studies are influenced by their choice of methodology. Similarly, the range of values for Australian isoprene emissions (both bottom-up and top-down) given in Table 3.1 should be discussed in more detail.What is it about the different emission models and inverse approaches  that lead to such a large range of values? Can the results of this work be understood simply in terms of the way the methodologies are applied, or has something genuinely new been learnt? In praise of Chapter 3, I really appreciated the detailed examination of uncertainties in the analysis, and in particular the thorough discussion of the role of the isoprene-HCHO yield and its implications for future work.</t>
   </si>
   <si>
     <t xml:space="preserve">I noticed several small apparent errors of understanding in Chapter 1 which the candidate should revisit while revising their thesis. For example, on page 3, the hydroperoxyl radical (HO 2 ) is referred to as “hydrogen dioxide”, a name which is never used in the relevant atmospheric chemistry literature. I was also not convinced by some aspects of the candidate’s description of ozone chemistry. For example the photolysis reaction of ozone in Equation Set 1.2 (page 4) is claimed to proceed at wavelengths less than 1180 nm. Does the candidate have a reference describing how quickly the reaction proceeds at such low photon energies? The absorption cross section for ozone photolysis used in the MCM (Master Chemical Mechanism) is only defined below 350 nm, with wavelength-dependent quantum yields for O( 1 D) and O( 3 P) below 350 nm (http://mcm.leeds.ac.uk/MCMv3.3.1/parameters/photolysis.htt). Significant amounts of ozone photolysis at lower photon energies would result in a much shorter lifetime for tropospheric ozone than predicted by the MCM (or any other model which I have used). Furthermore, the high abundance of “M” at lower altitudes is given as a reason for the existence of the ozone-layer, but M are actually required to stabilise ozone produced by photolysis in the stratosphere (Equation Set 1.2), where they are less abundant. The candidate should rethink and revise their text here.</t>
   </si>
   <si>
-    <t xml:space="preserve">Chemistry is not my strongest suit, so I do not pick up errors as readily as I should – thanks for pointing these out. </t>
+    <t xml:space="preserve">Chemistry is not my strongest suit, so I do not pick up errors as readily as I should – thanks for pointing these out. It appears that ozone is photolysed by light up to long wavelengths (~1100nm) however the cross section is orders of magnitude lower for wavelengths past 320nm (reference).</t>
   </si>
   <si>
     <t xml:space="preserve">Low wavelengths discussed in equation set 1.2 are updated to 350nm, updated sentence dealing with M abundance.</t>
@@ -335,8 +338,8 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -530,12 +533,14 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="257.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
@@ -549,7 +554,7 @@
     </row>
     <row r="31" customFormat="false" ht="200.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -564,15 +569,15 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="242.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,13 +592,13 @@
     </row>
     <row r="37" customFormat="false" ht="157.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,13 +613,13 @@
     </row>
     <row r="40" customFormat="false" ht="171.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,13 +634,13 @@
     </row>
     <row r="43" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added gaps in knowledge section to intro
</commit_message>
<xml_diff>
--- a/ResponseDocument.xlsx
+++ b/ResponseDocument.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">REVIEWER COMMENTS</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">The text switches from first to third person which becomes quite confusing as a reader. Given that the published work is in 3 rd person, I would suggest keeping the entire thesis the same.</t>
   </si>
   <si>
-    <t xml:space="preserve">I agree, or, there is aggreement</t>
+    <t xml:space="preserve">I agree</t>
   </si>
   <si>
     <r>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">The abstract needs some re-structuring. E.g. the aims come before the need/background. I suggest starting with the need/gaps, following with the aims/approach, and then following with key results. It is also lacking key contribution- why is this work important?</t>
   </si>
   <si>
+    <t xml:space="preserve">Thanks for the constructive feedback</t>
+  </si>
+  <si>
     <t xml:space="preserve">The abstract is somewhat reordered, with background more at the start and some additional notes on importance</t>
   </si>
   <si>
@@ -92,6 +95,12 @@
   </si>
   <si>
     <t xml:space="preserve">As with the Abstract, Chapter 1 could also do with some restructuring. The chapter contains a comprehensive introduction to ozone, and review of literature, however the gaps in knowledge that this thesis fills are hidden throughout and it is difficult to assess the context to the current study for some of the sections. Again, I suggest bearing in mind: need, gaps, aims/objectives structure while also introducing key background material and literature.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks again, instead of reorganising this chapter I hope summarising the knowledge gaps in a new section just before the aims addresses the main issue in your comment without breaking up the flow within the chapter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new section (1.7: Summary of gaps in knowledge) is added prior to Aims, dragging together the knowledge gaps into a single paragraph.</t>
   </si>
   <si>
     <t xml:space="preserve">Page 31- typo “..”</t>
@@ -170,7 +179,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -193,7 +202,7 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="15"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
@@ -206,7 +215,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="12"/>
       <name val="Cambria"/>
       <family val="1"/>
@@ -215,12 +223,6 @@
     <font>
       <vertAlign val="superscript"/>
       <sz val="12"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
@@ -307,11 +309,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -338,16 +340,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="18.55"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="81.9387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="56.1581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="54.9438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="80.9948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="55.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="54.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -361,35 +363,35 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="44.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
+    <row r="5" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="70.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -400,247 +402,253 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7"/>
+    <row r="7" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="87.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="86.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="138.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="143.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="225.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7"/>
+    <row r="17" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7"/>
+    <row r="18" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="72.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="104.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
+    <row r="20" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="72.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="104.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7"/>
+    <row r="22" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7"/>
+    <row r="24" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7"/>
+    <row r="25" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7"/>
+    <row r="27" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="398.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="200.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="311.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="380.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="157.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="242.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="171.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="260.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="87.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 1.7: summary of gaps in knowledge
</commit_message>
<xml_diff>
--- a/ResponseDocument.xlsx
+++ b/ResponseDocument.xlsx
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Thanks again, instead of reorganising this chapter I hope summarising the knowledge gaps in a new section just before the aims addresses the main issue in your comment without breaking up the flow within the chapter.</t>
   </si>
   <si>
-    <t xml:space="preserve">A new section (1.7: Summary of gaps in knowledge) is added prior to Aims, dragging together the knowledge gaps into a single paragraph.</t>
+    <t xml:space="preserve">A new section (1.7: Summary of gaps in knowledge) is added prior to Aims, dragging together the knowledge gaps into a single paragraph. Some now repeated information is then removed from the aims (now 1.8) and Australian and the southern hemisphere sections (1.6).</t>
   </si>
   <si>
     <t xml:space="preserve">Page 31- typo “..”</t>
@@ -340,7 +340,7 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
contributions in ch2, updated intro gaps ch1
</commit_message>
<xml_diff>
--- a/ResponseDocument.xlsx
+++ b/ResponseDocument.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t xml:space="preserve">REVIEWER COMMENTS</t>
   </si>
@@ -109,6 +109,12 @@
     <t xml:space="preserve">Chapter 2, called “Data and Modelling” details the datasets and modelling undertaken in the thesis, while also including results linked to Aim 2- calculation of vertical columns of HCHO. Once again, although the material presented is relevant, and the analyses appropriate, I am going to take issue with the structure of the chapter. As I read each section I found that although each contained interesting and relevant material, I kept having to go back to the explanation of the aims of the project on page 30 to see how and why that section fit within the thesis. This is also quite a long chapter. One suggestion would be to split the first half into a data and methods chapter, and the second half into results to meet Aim 2. I also suggest moving Fig 2.37 to earlier in the chapter, and then reefing to it throughout.</t>
   </si>
   <si>
+    <t xml:space="preserve">Both reviewers have suggested structural change to Chapter 2. I have followed the suggestions of Tim Butler as they slightly reduce the length of the chapter and may partly mitigate the issues mentioned here. Although I have moved Figure 2.37 as suggested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have implemented Tim Butler’s suggestions (first response for second reviewer in this document). and TODO: Fig 2.37 has been moved earlier, with references updated</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chapter 3 implements a top-down technique using satellite measurements of HCHO to calculate surface isoprene emissions. This chapter is clearly structured and easy to read and interpret. Well done. I have no suggestions for revisions to this chapter, beyond the use of 1 st person mentioned above, and would suggest that it is ready to submit to a journal if this hasn’t already taken place.</t>
   </si>
   <si>
@@ -130,7 +136,10 @@
     <t xml:space="preserve">The novel methodological aspects of the work are described in Chapter 2 of the thesis. I find this chapter somewhat confusing, because it appears to have three distinct purposes. Firstly, the chapter provides some general introductory material, which has substantial overlap with the introductory chapter. Secondly, the work done by the candidate to recalculate the OMI HCHO column measurements is described. These revised data are used in the subsequent chapter on isoprene inverse modelling (and presumably also by Lieschke et all, 2019). Thirdly, several filtering techniques are described, which it seems are only relevant for the isoprene inverse modelling work. I do understand the logic of including all of this material in a chapter called “Data and Modelling”, but I think a separation into distinct chapters would help the reader, and also make it clearer what the candidate has contributed. In particular, for the “middle part” of this text, it would be good to see a section similar to Section 4.9, in which the contributions of different workers (including the candidate) are clearly described. Subsequent work published (and even in preparation) using the new HCHO dataset could also be mentioned here, which would help to show how useful this work has been for colleagues and the wider community. Perhaps the work on filtering the HCHO columns (Section 2.7) could be merged into Chapter 3, especially if this will all be submitted as a standalone paper anyway.</t>
   </si>
   <si>
-    <t xml:space="preserve">Some intro from chapter 2 has been removed or replaced into chapter 1, with references added in chapter 2. Section 2.7: Filtering Data has been moved into Chapter 3 as subsection 3.2.3 under methods.</t>
+    <t xml:space="preserve">Thank you for the constructive feedback, I have done my best to handle each item mentioned here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some intro from chapter 2 has been removed or replaced into chapter 1, with references added in chapter 2. Section 2.7: Filtering Data has been moved into Chapter 3 as subsection 3.2.3 under methods. Contributions and acknowledgements has been added as a small section (2.8) prior to Data Access, listing summarily who did what for the chapter and where some work has been used outside the thesis.</t>
   </si>
   <si>
     <t xml:space="preserve">My main criticism of Chapter 3 is that the work is not described adequately in the context of previous studies. A top-down study by Bauwens et al. (2016) is mentioned in passing in Section 3.1.2, but almost no details are given. This study appears to be highly relevant, given that it seems to use an almost identical method. Chapter 3 must include a comparative discussion of the method used in this thesis and the method of Bauwens et al. (2016), and how the results of the two studies are influenced by their choice of methodology. Similarly, the range of values for Australian isoprene emissions (both bottom-up and top-down) given in Table 3.1 should be discussed in more detail.What is it about the different emission models and inverse approaches  that lead to such a large range of values? Can the results of this work be understood simply in terms of the way the methodologies are applied, or has something genuinely new been learnt? In praise of Chapter 3, I really appreciated the detailed examination of uncertainties in the analysis, and in particular the thorough discussion of the role of the isoprene-HCHO yield and its implications for future work.</t>
@@ -139,7 +148,7 @@
     <t xml:space="preserve">I noticed several small apparent errors of understanding in Chapter 1 which the candidate should revisit while revising their thesis. For example, on page 3, the hydroperoxyl radical (HO 2 ) is referred to as “hydrogen dioxide”, a name which is never used in the relevant atmospheric chemistry literature. I was also not convinced by some aspects of the candidate’s description of ozone chemistry. For example the photolysis reaction of ozone in Equation Set 1.2 (page 4) is claimed to proceed at wavelengths less than 1180 nm. Does the candidate have a reference describing how quickly the reaction proceeds at such low photon energies? The absorption cross section for ozone photolysis used in the MCM (Master Chemical Mechanism) is only defined below 350 nm, with wavelength-dependent quantum yields for O( 1 D) and O( 3 P) below 350 nm (http://mcm.leeds.ac.uk/MCMv3.3.1/parameters/photolysis.htt). Significant amounts of ozone photolysis at lower photon energies would result in a much shorter lifetime for tropospheric ozone than predicted by the MCM (or any other model which I have used). Furthermore, the high abundance of “M” at lower altitudes is given as a reason for the existence of the ozone-layer, but M are actually required to stabilise ozone produced by photolysis in the stratosphere (Equation Set 1.2), where they are less abundant. The candidate should rethink and revise their text here.</t>
   </si>
   <si>
-    <t xml:space="preserve">Chemistry is not my strongest suit, so I do not pick up errors as readily as I should – thanks for pointing these out. It appears that ozone is photolysed by light up to long wavelengths (~1100nm) however the cross section is orders of magnitude lower for wavelengths past 320nm (reference).</t>
+    <t xml:space="preserve">Chemistry is not my strongest suit, so I do not pick up errors as readily as I should – thanks for pointing these out. It appears that ozone is photolysed by light up to long wavelengths (~1100nm) however the cross section is orders of magnitude lower for wavelengths past 320nm (TODO: reference).</t>
   </si>
   <si>
     <t xml:space="preserve">Low wavelengths discussed in equation set 1.2 are updated to 350nm, updated sentence dealing with M abundance.</t>
@@ -179,7 +188,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -226,6 +235,12 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6.4"/>
+      <color rgb="FF3C3C3C"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -284,7 +299,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,6 +333,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,6 +349,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF3C3C3C"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -340,16 +419,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.55"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="80.9948979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="55.4795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="54.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="87.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="56.9642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="69.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,12 +546,16 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="225.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="208.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
@@ -486,10 +569,10 @@
     </row>
     <row r="19" customFormat="false" ht="104.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1"/>
     </row>
@@ -500,7 +583,7 @@
     </row>
     <row r="21" customFormat="false" ht="104.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -512,10 +595,10 @@
     </row>
     <row r="23" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1"/>
     </row>
@@ -531,7 +614,7 @@
     </row>
     <row r="26" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -541,13 +624,15 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="398.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="361.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C28" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,7 +647,7 @@
     </row>
     <row r="31" customFormat="false" ht="311.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -577,15 +662,15 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="380.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="361.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -600,13 +685,13 @@
     </row>
     <row r="37" customFormat="false" ht="242.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -621,13 +706,13 @@
     </row>
     <row r="40" customFormat="false" ht="260.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,13 +727,13 @@
     </row>
     <row r="43" customFormat="false" ht="87.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jenny's comments handled, except for bauwens comparison
</commit_message>
<xml_diff>
--- a/ResponseDocument.xlsx
+++ b/ResponseDocument.xlsx
@@ -97,10 +97,10 @@
     <t xml:space="preserve">As with the Abstract, Chapter 1 could also do with some restructuring. The chapter contains a comprehensive introduction to ozone, and review of literature, however the gaps in knowledge that this thesis fills are hidden throughout and it is difficult to assess the context to the current study for some of the sections. Again, I suggest bearing in mind: need, gaps, aims/objectives structure while also introducing key background material and literature.</t>
   </si>
   <si>
-    <t xml:space="preserve">Thanks again, instead of reorganising this chapter I hope summarising the knowledge gaps in a new section just before the aims addresses the main issue in your comment without breaking up the flow within the chapter.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A new section (1.7: Summary of gaps in knowledge) is added prior to Aims, dragging together the knowledge gaps into a single paragraph. Some now repeated information is then removed from the aims (now 1.8) and Australian and the southern hemisphere sections (1.6).</t>
+    <t xml:space="preserve">Thanks again. Due to the breadth of topics covered and the background required to understand the knowledge gaps, I have found it clearer to summarise the knowledge gaps in a new section just before the aims. I believe this addresses the main issue in this comment without breaking up the flow within the chapter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new section (1.7: Summary of gaps in knowledge) is added prior to Aims, bringing together the knowledge gaps into a single paragraph. Some now repeated information is then removed from the aims (now 1.8) and Australian and the southern hemisphere sections (1.6).</t>
   </si>
   <si>
     <t xml:space="preserve">Page 31- typo “..”</t>
@@ -109,10 +109,10 @@
     <t xml:space="preserve">Chapter 2, called “Data and Modelling” details the datasets and modelling undertaken in the thesis, while also including results linked to Aim 2- calculation of vertical columns of HCHO. Once again, although the material presented is relevant, and the analyses appropriate, I am going to take issue with the structure of the chapter. As I read each section I found that although each contained interesting and relevant material, I kept having to go back to the explanation of the aims of the project on page 30 to see how and why that section fit within the thesis. This is also quite a long chapter. One suggestion would be to split the first half into a data and methods chapter, and the second half into results to meet Aim 2. I also suggest moving Fig 2.37 to earlier in the chapter, and then reefing to it throughout.</t>
   </si>
   <si>
-    <t xml:space="preserve">Both reviewers have suggested structural change to Chapter 2. I have followed the suggestions of Tim Butler as they slightly reduce the length of the chapter and may partly mitigate the issues mentioned here. Although I have moved Figure 2.37 as suggested</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have implemented Tim Butler’s suggestions (first response for second reviewer in this document). Also Fig 2.37 has been moved from (now deleted) Section 2.8 to Section 2.6.1, along with discussion text (this is the OMHCHO recalculation outline section)</t>
+    <t xml:space="preserve">Both reviewers have suggested structural change to Chapter 2. I have followed the suggestions of Tim Butler as they reduce the length of the chapter and also mitigate the issues mentioned here. Although I have moved Figure 2.37 as suggested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have implemented Tim Butler’s suggestions (first response for second reviewer in this document). Also Fig 2.37 (now Fig. 2.21) has been moved from (now deleted) Section 2.8 to Section 2.6.1, along with discussion text (this is the OMHCHO recalculation outline section). Additionally the first paragraph in each subsection under 2.2.1 now explicitly state where the dataset is used within the thesis.</t>
   </si>
   <si>
     <t xml:space="preserve">Chapter 3 implements a top-down technique using satellite measurements of HCHO to calculate surface isoprene emissions. This chapter is clearly structured and easy to read and interpret. Well done. I have no suggestions for revisions to this chapter, beyond the use of 1 st person mentioned above, and would suggest that it is ready to submit to a journal if this hasn’t already taken place.</t>
@@ -124,10 +124,10 @@
     <t xml:space="preserve">Chapter 4 looks at stratospheric ozone intrusions and has been published in Atmospheric Chemistry and Physics. My only suggestion for this chapter would be to move the contribution of authors section to the beginning of the chapter, and to make clear how much of the work, perhaps as a percentage, can be contributed to the candidate.</t>
   </si>
   <si>
-    <t xml:space="preserve">This sounds reasonable, instead of changing the chapter I hope it is OK to COPY the first paragraph in the contributions into the foreword.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chapter 4 contributions from copied into foreword.</t>
+    <t xml:space="preserve">In order to maintain the same structure within each Chapter, and to additionally handle the first comment from T. Butler, I now provide a contributions section at the end of chapters 2 and 3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributions sections added to Chapter 2 and 3, with some additional text to address author contribution in the foreword of Chapter 4</t>
   </si>
   <si>
     <t xml:space="preserve">Chapter 5 is clearly written and does a good job of synthesizing the work. No revisions suggested.</t>
@@ -142,10 +142,10 @@
     <t xml:space="preserve">The novel methodological aspects of the work are described in Chapter 2 of the thesis. I find this chapter somewhat confusing, because it appears to have three distinct purposes. Firstly, the chapter provides some general introductory material, which has substantial overlap with the introductory chapter. Secondly, the work done by the candidate to recalculate the OMI HCHO column measurements is described. These revised data are used in the subsequent chapter on isoprene inverse modelling (and presumably also by Lieschke et all, 2019). Thirdly, several filtering techniques are described, which it seems are only relevant for the isoprene inverse modelling work. I do understand the logic of including all of this material in a chapter called “Data and Modelling”, but I think a separation into distinct chapters would help the reader, and also make it clearer what the candidate has contributed. In particular, for the “middle part” of this text, it would be good to see a section similar to Section 4.9, in which the contributions of different workers (including the candidate) are clearly described. Subsequent work published (and even in preparation) using the new HCHO dataset could also be mentioned here, which would help to show how useful this work has been for colleagues and the wider community. Perhaps the work on filtering the HCHO columns (Section 2.7) could be merged into Chapter 3, especially if this will all be submitted as a standalone paper anyway.</t>
   </si>
   <si>
-    <t xml:space="preserve">Thank you for the constructive feedback, I have done my best to handle each item mentioned here.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some intro from chapter 2 has been removed or replaced into chapter 1, with references added in chapter 2. Section 2.7: Filtering Data has been moved into Chapter 3 as subsection 3.2.3 under methods. Contributions and acknowledgements has been added as a small section (2.8) prior to Data Access, listing summarily who did what for the chapter and where some work has been used outside the thesis.</t>
+    <t xml:space="preserve">Thank you for the constructive feedback. I have made several modifications to address each item mentioned here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Several paragraphs from chapter 2, including some of the introduction, have been removed or replaced into chapter 1 . Section 2.7: Filtering Data has been moved into Chapter 3 as subsection 3.2.3 under methods. Contributions and acknowledgements has been added as a small section (new 2.7) prior to Data Access, listing summarily who did what for the chapter and where some work has been used outside the thesis.</t>
   </si>
   <si>
     <t xml:space="preserve">My main criticism of Chapter 3 is that the work is not described adequately in the context of previous studies. A top-down study by Bauwens et al. (2016) is mentioned in passing in Section 3.1.2, but almost no details are given. This study appears to be highly relevant, given that it seems to use an almost identical method. Chapter 3 must include a comparative discussion of the method used in this thesis and the method of Bauwens et al. (2016), and how the results of the two studies are influenced by their choice of methodology. Similarly, the range of values for Australian isoprene emissions (both bottom-up and top-down) given in Table 3.1 should be discussed in more detail. What is it about the different emission models and inverse approaches  that lead to such a large range of values? Can the results of this work be understood simply in terms of the way the methodologies are applied, or has something genuinely new been learnt? In praise of Chapter 3, I really appreciated the detailed examination of uncertainties in the analysis, and in particular the thorough discussion of the role of the isoprene-HCHO yield and its implications for future work.</t>
@@ -160,19 +160,19 @@
     <t xml:space="preserve">I noticed several small apparent errors of understanding in Chapter 1 which the candidate should revisit while revising their thesis. For example, on page 3, the hydroperoxyl radical (HO 2 ) is referred to as “hydrogen dioxide”, a name which is never used in the relevant atmospheric chemistry literature. I was also not convinced by some aspects of the candidate’s description of ozone chemistry. For example the photolysis reaction of ozone in Equation Set 1.2 (page 4) is claimed to proceed at wavelengths less than 1180 nm. Does the candidate have a reference describing how quickly the reaction proceeds at such low photon energies? The absorption cross section for ozone photolysis used in the MCM (Master Chemical Mechanism) is only defined below 350 nm, with wavelength-dependent quantum yields for O( 1 D) and O( 3 P) below 350 nm (http://mcm.leeds.ac.uk/MCMv3.3.1/parameters/photolysis.htt). Significant amounts of ozone photolysis at lower photon energies would result in a much shorter lifetime for tropospheric ozone than predicted by the MCM (or any other model which I have used). Furthermore, the high abundance of “M” at lower altitudes is given as a reason for the existence of the ozone-layer, but M are actually required to stabilise ozone produced by photolysis in the stratosphere (Equation Set 1.2), where they are less abundant. The candidate should rethink and revise their text here.</t>
   </si>
   <si>
-    <t xml:space="preserve">Chemistry is not my strongest suit, so I do not pick up errors as readily as I should – thanks for pointing these out. You are right that the ozone cross section is orders of magnitude lower for wavelengths past 320nm. In this work it is perhaps only relevant to talk about what wavelengths are commonly modelled so I have made the changes as you suggest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low wavelengths discussed in equation set 1.2 are updated to 350nm, updated sentence dealing with M abundance.</t>
+    <t xml:space="preserve">Thanks for pointing these out. You are right that the ozone cross section is orders of magnitude lower for wavelengths past 320nm. In this work it is perhaps only relevant to talk about what wavelengths are commonly modelled so I have made the changes as you suggest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Hydrogen dioxide" has been replaced with "hydroperoxyl radical". Low wavelengths discussed in equation set 1.2 are updated to 350nm, updated sentence dealing with M abundance.</t>
   </si>
   <si>
     <t xml:space="preserve">I also think that the candidate should give a better overview of the different kinds of sources of VOC in Section 1.3. The candidate primarily focuses on biogenic isoprene, which is reasonable given the focus of the thesis, but anthropogenic and pyrogenic VOC are barely mentioned, and not until later in the text. Also, “reactivity” is listed as one of the fundamental properties of VOC near the beginning of Section 1.3, but I miss some discussion about what determines the reactivity of different VOC, and what this means for their atmospheric lifetimes. This is especially important, since the atmospheric lifetimes of both isoprene and HCHO are important concepts which are drawn upon in several places later in the thesis.</t>
   </si>
   <si>
-    <t xml:space="preserve">Thanks, it is good to have feedback on what may be missing from the intro. Instead of shuffling pyro and anthro emissions into the intro, I hope it is ok to just mention that they are important and point to the sections where I deal with them specifically.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Added to third paragraph in 1.3: “Other major emission sources of VOC (anthropogenic and pyrogenic) are also important.” and “This thesis mostly focuses on biogenic emissions, with influences from pyrogenic and anthropogenic emissions removed (Section 2.7)”. Added to first paragraph in 1.3: “These properties are largely dictated by the chemical makeup of the individual compounds. A compound's atmospheric lifetime is strongly related to its reactivity (and the concentration of reactants), with more reactive compounds having shorter atmospheric lifetimes.”</t>
+    <t xml:space="preserve">This is a good point. Pyrogenic and anthropogenic VOC sources are now mentioned earlier in 1.3, when biogenic sources are first introduced. The fact that these sources are not important for this thesis is also noted early in this section so that the rationale for the focus on biogenic sources is clearer. The text on reactivity has also been expanded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added to third paragraph in 1.3: “Other major emission sources of VOC (anthropogenic and pyrogenic) are also important.” and “This thesis mostly focuses on biogenic emissions, with influences from pyrogenic and anthropogenic emissions removed (Section 2.7)”. Added to first paragraph in 1.3: “These properties are largely dictated by the chemical makeup and structure of the individual compounds. A compound's atmospheric lifetime is strongly related to its reactivity (and the concentration of reactants), with more reactive compounds having shorter atmospheric lifetimes.”</t>
   </si>
   <si>
     <t xml:space="preserve">Given their importance in the thesis, I would also like to see more understanding of biogenic isoprene emissions demonstrated by the candidate in Chapter 1, especially how they are modelled, and the basis (or lack thereof) that this emissions modelling has in actual measured data. BVOC emission models, specifically MEGAN, are mentioned in several places in the thesis. In many of these cases literature references are given, and particular aspects of the potential shortcomings in these models are described, such as a poor representation of soil moisture, or an over-reliance on measurements from younger trees. Instead of scattering this information throughout the thesis it should be collected in one place where the candidate can demonstrate an understanding of how these models work and what their known shortcomings are. The results in subsequent chapters can then be related back to the material from the introduction</t>
@@ -187,10 +187,10 @@
     <t xml:space="preserve">As a matter of style, tables and figures should not be presented in the conclusions chapter. Figure 5.2 is particularly superfluous, since it is exactly the same as Figure 3.7</t>
   </si>
   <si>
-    <t xml:space="preserve">OK it seems fair to have no figures or new material in the conclusions, however I would like to keep the table as it is much clearer than a long list of numbers that I would have otherwise.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Figure 5.1 moved into Chapter 3 results as Figure 3.21, with some text added there, and some text replaced in the Conclusions chapter. Figure 5.2 removed, sentence now references original figure.</t>
+    <t xml:space="preserve">OK, thanks for pointing this out.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 5.1 moved into Chapter 3 results as Figure 3.21, with some text added there, and some text replaced in the Conclusions chapter. Figure 5.2 removed, sentence now references original figure. Table 5.1 is also removed to Chapter 3 results with some discussion added as Table 3.7.</t>
   </si>
 </sst>
 </file>
@@ -200,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -254,6 +254,11 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -312,7 +317,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -350,6 +355,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -432,16 +441,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="86.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="56.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="68.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.1785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="55.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="68.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,7 +538,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="116.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -559,7 +568,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="182.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="182.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -598,10 +607,10 @@
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -641,7 +650,7 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="331.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
         <v>30</v>
       </c>
@@ -683,7 +692,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="331.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
         <v>36</v>
       </c>
@@ -704,7 +713,7 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="166.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="182.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
         <v>39</v>
       </c>
@@ -746,7 +755,7 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="83.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
handled Jenny's feedback on tracked changes
</commit_message>
<xml_diff>
--- a/ResponseDocument.xlsx
+++ b/ResponseDocument.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">The text switches from first to third person which becomes quite confusing as a reader. Given that the published work is in 3 rd person, I would suggest keeping the entire thesis the same.</t>
   </si>
   <si>
-    <t xml:space="preserve">I agree</t>
+    <t xml:space="preserve">Thanks for the feedback, I agree and would like to keep confusion to a minimum</t>
   </si>
   <si>
     <r>
@@ -151,16 +151,16 @@
     <t xml:space="preserve">My main criticism of Chapter 3 is that the work is not described adequately in the context of previous studies. A top-down study by Bauwens et al. (2016) is mentioned in passing in Section 3.1.2, but almost no details are given. This study appears to be highly relevant, given that it seems to use an almost identical method. Chapter 3 must include a comparative discussion of the method used in this thesis and the method of Bauwens et al. (2016), and how the results of the two studies are influenced by their choice of methodology. Similarly, the range of values for Australian isoprene emissions (both bottom-up and top-down) given in Table 3.1 should be discussed in more detail. What is it about the different emission models and inverse approaches  that lead to such a large range of values? Can the results of this work be understood simply in terms of the way the methodologies are applied, or has something genuinely new been learnt? In praise of Chapter 3, I really appreciated the detailed examination of uncertainties in the analysis, and in particular the thorough discussion of the role of the isoprene-HCHO yield and its implications for future work.</t>
   </si>
   <si>
-    <t xml:space="preserve">Thanks for these comments. Bauwens et al. 2016 do a similar analysis however their implementation, a priori inventory, and chemical model are all different. I’m of the opinion that the major differences in results arise more from the differences between chemical models than anything else. The fact that we see similar results (reduction of a priori) is encouraging and I’ve hopefully now added that message to the text. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Where Bauwens et al. 2016 is introduced in 3.1.2 now includes a reference to where I compare my results with theirs. The comparison (final paragraph of 3.3.1) has been extended, providing further comparative discussion around results, methodology, and potential influences. A figure and its analysis has been moved to earlier in the section so that the paragraph is not too long.</t>
+    <t xml:space="preserve">Thanks for these comments. Bauwens et al. 2016 do a similar analysis however their implementation, a priori inventory, and chemical model are all different. This is now discussed in the text. I’m of the opinion that the major differences in results arise more from the differences between chemical models than anything else. The fact that we see similar results (reduction of a priori) is encouraging and I’ve hopefully now added that message to the text. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where Bauwens et al. 2016 is introduced in 3.1.2 now includes a reference to where I compare my results with theirs. I have added a new subsection 3.3.1.1: comparison to other estimates, providing further comparative discussion around results, methodology, and potential influences. Some text has been moved to accommodate this.</t>
   </si>
   <si>
     <t xml:space="preserve">I noticed several small apparent errors of understanding in Chapter 1 which the candidate should revisit while revising their thesis. For example, on page 3, the hydroperoxyl radical (HO 2 ) is referred to as “hydrogen dioxide”, a name which is never used in the relevant atmospheric chemistry literature. I was also not convinced by some aspects of the candidate’s description of ozone chemistry. For example the photolysis reaction of ozone in Equation Set 1.2 (page 4) is claimed to proceed at wavelengths less than 1180 nm. Does the candidate have a reference describing how quickly the reaction proceeds at such low photon energies? The absorption cross section for ozone photolysis used in the MCM (Master Chemical Mechanism) is only defined below 350 nm, with wavelength-dependent quantum yields for O( 1 D) and O( 3 P) below 350 nm (http://mcm.leeds.ac.uk/MCMv3.3.1/parameters/photolysis.htt). Significant amounts of ozone photolysis at lower photon energies would result in a much shorter lifetime for tropospheric ozone than predicted by the MCM (or any other model which I have used). Furthermore, the high abundance of “M” at lower altitudes is given as a reason for the existence of the ozone-layer, but M are actually required to stabilise ozone produced by photolysis in the stratosphere (Equation Set 1.2), where they are less abundant. The candidate should rethink and revise their text here.</t>
   </si>
   <si>
-    <t xml:space="preserve">Thanks for pointing these out. You are right that the ozone cross section is orders of magnitude lower for wavelengths past 320nm. In this work it is perhaps only relevant to talk about what wavelengths are commonly modelled so I have made the changes as you suggest</t>
+    <t xml:space="preserve">Thanks for pointing these out. You are right that the ozone cross section is orders of magnitude lower for wavelengths past 320nm. In this work it is only relevant to talk about what wavelengths are commonly modelled so I have made the changes as you suggest</t>
   </si>
   <si>
     <t xml:space="preserve">"Hydrogen dioxide" has been replaced with "hydroperoxyl radical". Low wavelengths discussed in equation set 1.2 are updated to 350nm, updated sentence dealing with M abundance.</t>
@@ -257,8 +257,10 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -358,8 +360,8 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -375,7 +377,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFC00000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -439,18 +441,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.1785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="55.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="68.0357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="3" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="74.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="50.1530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="48.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="65.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,7 +479,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="50.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -492,7 +495,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="50.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="83.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -508,7 +511,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="83.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -538,7 +541,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="133.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -568,7 +571,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="182.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="215.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -589,7 +592,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="100.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="116.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -603,14 +606,14 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="83.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="100.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -650,7 +653,7 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="397.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
         <v>30</v>
       </c>
@@ -671,7 +674,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="265.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
         <v>33</v>
       </c>
@@ -681,6 +684,7 @@
       <c r="C31" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
@@ -692,7 +696,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="380.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
         <v>36</v>
       </c>
@@ -713,7 +717,7 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="182.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="248.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
         <v>39</v>
       </c>
@@ -734,7 +738,7 @@
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="215.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="248.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
         <v>42</v>
       </c>
@@ -755,7 +759,7 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="83.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="116.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
         <v>45</v>
       </c>

</xml_diff>